<commit_message>
Summarize management prevalance by fire; exclude units not completed
</commit_message>
<xml_diff>
--- a/data/site-selection/manual-summaries/mgmt_type_breakdown_stats.xlsx
+++ b/data/site-selection/manual-summaries/mgmt_type_breakdown_stats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
   <si>
     <t>2007 Antelope</t>
   </si>
@@ -137,9 +137,6 @@
     <t>fire will probably work; need snag retention plot locations to know for sure, predominantely released, plt yrs 1-2</t>
   </si>
   <si>
-    <t>only about 6 plots each of plt. Yr. 3 and plt. Yr. 4</t>
-  </si>
-  <si>
     <t>1987 clark</t>
   </si>
   <si>
@@ -174,6 +171,15 @@
   </si>
   <si>
     <t>had prep</t>
+  </si>
+  <si>
+    <t>also yr 2 in smaller elev. range</t>
+  </si>
+  <si>
+    <t>only about 8 plots each of plt. Yr. 3 and plt. Yr. 4</t>
+  </si>
+  <si>
+    <t>also plt. Yr. 3 in smaller elev. range</t>
   </si>
 </sst>
 </file>
@@ -585,10 +591,10 @@
   <dimension ref="A1:O33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E25" sqref="E21:E25"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -634,13 +640,13 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="N1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -723,7 +729,7 @@
         <v>2</v>
       </c>
       <c r="N5" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O5">
         <v>1</v>
@@ -738,7 +744,7 @@
         <v>28</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>32</v>
@@ -759,7 +765,7 @@
         <v>114</v>
       </c>
       <c r="D7" s="3">
-        <v>125</v>
+        <v>300</v>
       </c>
       <c r="G7" s="3"/>
       <c r="J7">
@@ -803,7 +809,7 @@
         <v>4000</v>
       </c>
       <c r="D9">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="G9" s="3"/>
       <c r="J9" s="5">
@@ -824,8 +830,8 @@
       <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4">
-        <v>2</v>
+      <c r="D10" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>32</v>
@@ -852,7 +858,10 @@
         <v>27</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>40</v>
+        <v>53</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -978,7 +987,7 @@
         <v>33</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -989,11 +998,11 @@
         <v>27</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J20" s="8"/>
       <c r="L20" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1093,6 +1102,12 @@
       <c r="F25" s="8" t="s">
         <v>31</v>
       </c>
+      <c r="K25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="15" t="s">
@@ -1129,7 +1144,7 @@
         <v>35</v>
       </c>
       <c r="M29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1146,31 +1161,31 @@
         <v>38</v>
       </c>
       <c r="E32" t="s">
+        <v>46</v>
+      </c>
+      <c r="F32" t="s">
         <v>47</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" t="s">
         <v>48</v>
       </c>
-      <c r="G32" t="s">
-        <v>47</v>
-      </c>
-      <c r="H32" t="s">
+      <c r="I32" t="s">
+        <v>50</v>
+      </c>
+      <c r="J32" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" t="s">
+        <v>46</v>
+      </c>
+      <c r="L32" t="s">
         <v>49</v>
       </c>
-      <c r="I32" t="s">
-        <v>51</v>
-      </c>
-      <c r="J32" t="s">
-        <v>47</v>
-      </c>
-      <c r="K32" t="s">
-        <v>47</v>
-      </c>
-      <c r="L32" t="s">
-        <v>50</v>
-      </c>
       <c r="M32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Break down by release timing; helicopter salvage is separate category
</commit_message>
<xml_diff>
--- a/data/site-selection/manual-summaries/mgmt_type_breakdown_stats.xlsx
+++ b/data/site-selection/manual-summaries/mgmt_type_breakdown_stats.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>2007 Antelope</t>
   </si>
@@ -107,9 +107,6 @@
     <t>2,3</t>
   </si>
   <si>
-    <t>much wider elev. range for yr. 2 planting only</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>2,3,4</t>
   </si>
   <si>
-    <t>3,4,5</t>
-  </si>
-  <si>
     <t>plt years</t>
   </si>
   <si>
@@ -176,17 +170,26 @@
     <t>also yr 2 in smaller elev. range</t>
   </si>
   <si>
-    <t>only about 8 plots each of plt. Yr. 3 and plt. Yr. 4</t>
-  </si>
-  <si>
     <t>also plt. Yr. 3 in smaller elev. range</t>
+  </si>
+  <si>
+    <t>only about 5 plots of plt yr 4; release was post-yr10</t>
+  </si>
+  <si>
+    <t>36+</t>
+  </si>
+  <si>
+    <t>only about 8 plots each of plt. Yr. 4.; wider elev. range in plt. Yr. 2 only</t>
+  </si>
+  <si>
+    <t>somewhat wider elev. range for yr. 2 planting only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -202,8 +205,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -213,6 +233,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -268,7 +300,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -287,6 +318,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +635,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,17 +681,17 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="N1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B2" t="s">
@@ -665,7 +706,7 @@
       <c r="G2">
         <v>21</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="19">
         <v>426</v>
       </c>
       <c r="O2">
@@ -673,7 +714,7 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
+      <c r="A3" s="16"/>
       <c r="B3" t="s">
         <v>16</v>
       </c>
@@ -686,7 +727,7 @@
       <c r="G3">
         <v>200</v>
       </c>
-      <c r="N3" s="9">
+      <c r="N3" s="19">
         <v>250</v>
       </c>
       <c r="O3">
@@ -694,7 +735,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="17"/>
+      <c r="A4" s="16"/>
       <c r="B4" t="s">
         <v>17</v>
       </c>
@@ -707,7 +748,7 @@
       <c r="G4">
         <v>2000</v>
       </c>
-      <c r="N4" s="9">
+      <c r="N4" s="19">
         <v>2500</v>
       </c>
       <c r="O4">
@@ -715,9 +756,9 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5" s="17"/>
+      <c r="A5" s="16"/>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" s="9">
         <v>3</v>
@@ -728,34 +769,34 @@
       <c r="G5">
         <v>2</v>
       </c>
-      <c r="N5" s="10" t="s">
-        <v>41</v>
+      <c r="N5" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="18"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>52</v>
+      <c r="D6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N6" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="N6" s="20"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="15" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
@@ -771,15 +812,15 @@
       <c r="J7">
         <v>36</v>
       </c>
-      <c r="K7">
-        <v>36</v>
+      <c r="K7" s="21" t="s">
+        <v>53</v>
       </c>
       <c r="O7" s="3">
         <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="17"/>
+      <c r="A8" s="16"/>
       <c r="B8" t="s">
         <v>16</v>
       </c>
@@ -793,7 +834,7 @@
       <c r="J8">
         <v>300</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="24">
         <v>200</v>
       </c>
       <c r="O8">
@@ -801,7 +842,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="17"/>
+      <c r="A9" s="16"/>
       <c r="B9" t="s">
         <v>17</v>
       </c>
@@ -815,7 +856,7 @@
       <c r="J9" s="5">
         <v>4000</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="21">
         <v>3500</v>
       </c>
       <c r="O9">
@@ -823,9 +864,9 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>25</v>
@@ -834,10 +875,10 @@
         <v>29</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -845,38 +886,38 @@
       <c r="J10" s="4">
         <v>3</v>
       </c>
-      <c r="K10" s="7" t="s">
-        <v>33</v>
+      <c r="K10" s="25" t="s">
+        <v>32</v>
       </c>
       <c r="O10">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>53</v>
+      <c r="K11" s="23" t="s">
+        <v>54</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="12">
         <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="17"/>
+      <c r="A13" s="16"/>
       <c r="B13" t="s">
         <v>16</v>
       </c>
@@ -885,7 +926,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="17"/>
+      <c r="A14" s="16"/>
       <c r="B14" t="s">
         <v>17</v>
       </c>
@@ -894,16 +935,16 @@
       </c>
     </row>
     <row r="15" spans="1:15" s="2" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="19"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B16" t="s">
@@ -913,10 +954,10 @@
         <v>44</v>
       </c>
       <c r="I16" s="9"/>
-      <c r="J16" s="9">
+      <c r="J16" s="19">
         <v>51</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="21">
         <v>249</v>
       </c>
       <c r="M16">
@@ -924,7 +965,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A17" s="17"/>
+      <c r="A17" s="16"/>
       <c r="B17" t="s">
         <v>16</v>
       </c>
@@ -932,10 +973,10 @@
         <v>400</v>
       </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="10">
+      <c r="J17" s="26">
         <v>700</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="21">
         <v>100</v>
       </c>
       <c r="M17">
@@ -943,7 +984,7 @@
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A18" s="17"/>
+      <c r="A18" s="16"/>
       <c r="B18" t="s">
         <v>17</v>
       </c>
@@ -951,10 +992,10 @@
         <v>3000</v>
       </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="10">
+      <c r="J18" s="28">
         <v>4000</v>
       </c>
-      <c r="L18" s="9">
+      <c r="L18" s="21">
         <v>500</v>
       </c>
       <c r="M18">
@@ -962,29 +1003,29 @@
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A19" s="17"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4">
         <v>3</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="11" t="s">
-        <v>33</v>
+      <c r="I19" s="12"/>
+      <c r="J19" s="27" t="s">
+        <v>32</v>
       </c>
       <c r="K19" s="4"/>
-      <c r="L19" s="10" t="s">
-        <v>33</v>
+      <c r="L19" s="22" t="s">
+        <v>32</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>29</v>
@@ -993,20 +1034,20 @@
       <c r="O19" s="4"/>
     </row>
     <row r="20" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="18"/>
+      <c r="A20" s="17"/>
       <c r="B20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="J20" s="8"/>
-      <c r="L20" s="8" t="s">
-        <v>42</v>
+        <v>49</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="L20" s="23" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
@@ -1018,8 +1059,8 @@
       <c r="F21" s="9">
         <v>25</v>
       </c>
-      <c r="G21">
-        <v>19</v>
+      <c r="G21" s="21">
+        <v>30</v>
       </c>
       <c r="J21" s="3">
         <v>62</v>
@@ -1029,7 +1070,7 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="17"/>
+      <c r="A22" s="16"/>
       <c r="B22" t="s">
         <v>16</v>
       </c>
@@ -1039,7 +1080,7 @@
       <c r="F22" s="10">
         <v>600</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="21">
         <v>200</v>
       </c>
       <c r="J22" s="6">
@@ -1050,7 +1091,7 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A23" s="17"/>
+      <c r="A23" s="16"/>
       <c r="B23" t="s">
         <v>17</v>
       </c>
@@ -1060,7 +1101,7 @@
       <c r="F23" s="10">
         <v>5000</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="21">
         <v>3000</v>
       </c>
       <c r="J23" s="5">
@@ -1071,9 +1112,9 @@
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A24" s="17"/>
+      <c r="A24" s="16"/>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>25</v>
@@ -1081,36 +1122,39 @@
       <c r="F24" s="9">
         <v>2</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J24">
-        <v>2</v>
+      <c r="G24" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="J24" t="s">
+        <v>29</v>
       </c>
       <c r="K24">
         <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="E25" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>31</v>
+      <c r="G25" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B26" t="s">
@@ -1121,7 +1165,7 @@
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
         <v>16</v>
       </c>
@@ -1130,7 +1174,7 @@
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
+      <c r="A28" s="14"/>
       <c r="B28" t="s">
         <v>17</v>
       </c>
@@ -1139,12 +1183,12 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
+      <c r="A29" s="14"/>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="M29" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -1158,48 +1202,48 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H32" t="s">
         <v>46</v>
       </c>
-      <c r="F32" t="s">
+      <c r="I32" t="s">
+        <v>48</v>
+      </c>
+      <c r="J32" t="s">
+        <v>44</v>
+      </c>
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+      <c r="L32" t="s">
         <v>47</v>
       </c>
-      <c r="G32" t="s">
-        <v>46</v>
-      </c>
-      <c r="H32" t="s">
-        <v>48</v>
-      </c>
-      <c r="I32" t="s">
-        <v>50</v>
-      </c>
-      <c r="J32" t="s">
-        <v>46</v>
-      </c>
-      <c r="K32" t="s">
-        <v>46</v>
-      </c>
-      <c r="L32" t="s">
-        <v>49</v>
-      </c>
       <c r="M32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H33" t="s">
+        <v>35</v>
+      </c>
+      <c r="I33" t="s">
         <v>37</v>
       </c>
-      <c r="I33" t="s">
-        <v>39</v>
-      </c>
       <c r="J33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>